<commit_message>
cleaning out unused code, fixing comments
</commit_message>
<xml_diff>
--- a/hdcntfunc.xlsx
+++ b/hdcntfunc.xlsx
@@ -25,6 +25,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>employe_num</t>
+  </si>
+  <si>
+    <t>employee_name</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>doe</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
     <t>1000</t>
   </si>
   <si>
@@ -35,27 +56,6 @@
   </si>
   <si>
     <t>kavi</t>
-  </si>
-  <si>
-    <t>division</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>employe_num</t>
-  </si>
-  <si>
-    <t>employee_name</t>
-  </si>
-  <si>
-    <t>manager</t>
-  </si>
-  <si>
-    <t>doe</t>
-  </si>
-  <si>
-    <t>project</t>
   </si>
   <si>
     <t>Tot. Hours</t>
@@ -634,43 +634,43 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="n">
-        <v>841596</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="n">
-        <v>46</v>
-      </c>
-      <c r="G1" t="n">
-        <v>114</v>
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>841596</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
         <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2" t="n">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -694,25 +694,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>57</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
@@ -873,25 +873,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -952,25 +952,25 @@
     <row r="4" spans="1:10"/>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -996,7 +996,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
         <v>21</v>
@@ -1008,25 +1008,25 @@
     <row r="7" spans="1:10"/>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G8" t="s">
         <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -1243,25 +1243,25 @@
     <row r="17" spans="1:10"/>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="F18" t="s">
         <v>5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="G18" t="s">
         <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -1322,25 +1322,25 @@
     <row r="21" spans="1:10"/>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="F22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="G22" t="s">
         <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
-        <v>10</v>
       </c>
       <c r="H22" t="s">
         <v>11</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
         <v>32</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1562,25 +1562,25 @@
     <row r="32" spans="1:10"/>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
+      <c r="F33" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
+      <c r="G33" t="s">
         <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
-        <v>10</v>
       </c>
       <c r="H33" t="s">
         <v>11</v>
@@ -1594,7 +1594,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
         <v>42</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
         <v>42</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
         <v>42</v>
@@ -1664,25 +1664,25 @@
     <row r="37" spans="1:10"/>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
+      <c r="F38" t="s">
         <v>5</v>
       </c>
-      <c r="C38" t="s">
+      <c r="G38" t="s">
         <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" t="s">
-        <v>10</v>
       </c>
       <c r="H38" t="s">
         <v>11</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
@@ -1720,25 +1720,25 @@
     <row r="40" spans="1:10"/>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
+      <c r="F41" t="s">
         <v>5</v>
       </c>
-      <c r="C41" t="s">
+      <c r="G41" t="s">
         <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" t="s">
-        <v>10</v>
       </c>
       <c r="H41" t="s">
         <v>11</v>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
         <v>48</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
         <v>48</v>
@@ -1822,25 +1822,25 @@
     <row r="45" spans="1:10"/>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
+      <c r="F46" t="s">
         <v>5</v>
       </c>
-      <c r="C46" t="s">
+      <c r="G46" t="s">
         <v>6</v>
-      </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" t="s">
-        <v>8</v>
-      </c>
-      <c r="F46" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" t="s">
-        <v>10</v>
       </c>
       <c r="H46" t="s">
         <v>11</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
         <v>52</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
         <v>52</v>
@@ -1901,25 +1901,25 @@
     <row r="49" spans="1:10"/>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
         <v>4</v>
       </c>
-      <c r="B50" t="s">
+      <c r="F50" t="s">
         <v>5</v>
       </c>
-      <c r="C50" t="s">
+      <c r="G50" t="s">
         <v>6</v>
-      </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" t="s">
-        <v>10</v>
       </c>
       <c r="H50" t="s">
         <v>11</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
         <v>55</v>
@@ -1957,25 +1957,25 @@
     <row r="52" spans="1:10"/>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
         <v>4</v>
       </c>
-      <c r="B53" t="s">
+      <c r="F53" t="s">
         <v>5</v>
       </c>
-      <c r="C53" t="s">
+      <c r="G53" t="s">
         <v>6</v>
-      </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" t="s">
-        <v>9</v>
-      </c>
-      <c r="G53" t="s">
-        <v>10</v>
       </c>
       <c r="H53" t="s">
         <v>11</v>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
         <v>57</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
         <v>57</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
         <v>57</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
         <v>57</v>
@@ -2082,25 +2082,25 @@
     <row r="58" spans="1:10"/>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
         <v>4</v>
       </c>
-      <c r="B59" t="s">
+      <c r="F59" t="s">
         <v>5</v>
       </c>
-      <c r="C59" t="s">
+      <c r="G59" t="s">
         <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" t="s">
-        <v>8</v>
-      </c>
-      <c r="F59" t="s">
-        <v>9</v>
-      </c>
-      <c r="G59" t="s">
-        <v>10</v>
       </c>
       <c r="H59" t="s">
         <v>11</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B60" t="s">
         <v>63</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B61" t="s">
         <v>63</v>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B62" t="s">
         <v>63</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B63" t="s">
         <v>63</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
@@ -2230,25 +2230,25 @@
     <row r="65" spans="1:10"/>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
         <v>4</v>
       </c>
-      <c r="B66" t="s">
+      <c r="F66" t="s">
         <v>5</v>
       </c>
-      <c r="C66" t="s">
+      <c r="G66" t="s">
         <v>6</v>
-      </c>
-      <c r="D66" t="s">
-        <v>7</v>
-      </c>
-      <c r="E66" t="s">
-        <v>8</v>
-      </c>
-      <c r="F66" t="s">
-        <v>9</v>
-      </c>
-      <c r="G66" t="s">
-        <v>10</v>
       </c>
       <c r="H66" t="s">
         <v>11</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B67" t="s">
         <v>70</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B68" t="s">
         <v>70</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B69" t="s">
         <v>70</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B70" t="s">
         <v>70</v>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B71" t="s">
         <v>70</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B72" t="s">
         <v>70</v>
@@ -2401,25 +2401,25 @@
     <row r="73" spans="1:10"/>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" t="s">
         <v>4</v>
       </c>
-      <c r="B74" t="s">
+      <c r="F74" t="s">
         <v>5</v>
       </c>
-      <c r="C74" t="s">
+      <c r="G74" t="s">
         <v>6</v>
-      </c>
-      <c r="D74" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" t="s">
-        <v>8</v>
-      </c>
-      <c r="F74" t="s">
-        <v>9</v>
-      </c>
-      <c r="G74" t="s">
-        <v>10</v>
       </c>
       <c r="H74" t="s">
         <v>11</v>
@@ -2433,7 +2433,7 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B75" t="s">
         <v>77</v>
@@ -2457,25 +2457,25 @@
     <row r="76" spans="1:10"/>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
         <v>4</v>
       </c>
-      <c r="B77" t="s">
+      <c r="F77" t="s">
         <v>5</v>
       </c>
-      <c r="C77" t="s">
+      <c r="G77" t="s">
         <v>6</v>
-      </c>
-      <c r="D77" t="s">
-        <v>7</v>
-      </c>
-      <c r="E77" t="s">
-        <v>8</v>
-      </c>
-      <c r="F77" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" t="s">
-        <v>10</v>
       </c>
       <c r="H77" t="s">
         <v>11</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B78" t="s">
         <v>80</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B79" t="s">
         <v>80</v>
@@ -2536,25 +2536,25 @@
     <row r="80" spans="1:10"/>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" t="s">
         <v>4</v>
       </c>
-      <c r="B81" t="s">
+      <c r="F81" t="s">
         <v>5</v>
       </c>
-      <c r="C81" t="s">
+      <c r="G81" t="s">
         <v>6</v>
-      </c>
-      <c r="D81" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" t="s">
-        <v>8</v>
-      </c>
-      <c r="F81" t="s">
-        <v>9</v>
-      </c>
-      <c r="G81" t="s">
-        <v>10</v>
       </c>
       <c r="H81" t="s">
         <v>11</v>
@@ -2568,19 +2568,19 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C82" t="n">
         <v>841596</v>
       </c>
       <c r="D82" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E82" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F82" t="n">
         <v>46</v>
@@ -2592,25 +2592,25 @@
     <row r="83" spans="1:10"/>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" t="s">
         <v>4</v>
       </c>
-      <c r="B84" t="s">
+      <c r="F84" t="s">
         <v>5</v>
       </c>
-      <c r="C84" t="s">
+      <c r="G84" t="s">
         <v>6</v>
-      </c>
-      <c r="D84" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84" t="s">
-        <v>9</v>
-      </c>
-      <c r="G84" t="s">
-        <v>10</v>
       </c>
       <c r="H84" t="s">
         <v>11</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B85" t="s">
         <v>83</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B86" t="s">
         <v>83</v>
@@ -2671,25 +2671,25 @@
     <row r="87" spans="1:10"/>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>3</v>
+      </c>
+      <c r="E88" t="s">
         <v>4</v>
       </c>
-      <c r="B88" t="s">
+      <c r="F88" t="s">
         <v>5</v>
       </c>
-      <c r="C88" t="s">
+      <c r="G88" t="s">
         <v>6</v>
-      </c>
-      <c r="D88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E88" t="s">
-        <v>8</v>
-      </c>
-      <c r="F88" t="s">
-        <v>9</v>
-      </c>
-      <c r="G88" t="s">
-        <v>10</v>
       </c>
       <c r="H88" t="s">
         <v>11</v>
@@ -2703,25 +2703,25 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>3</v>
+      </c>
+      <c r="E89" t="s">
         <v>4</v>
       </c>
-      <c r="B89" t="s">
+      <c r="F89" t="s">
         <v>5</v>
       </c>
-      <c r="C89" t="s">
+      <c r="G89" t="s">
         <v>6</v>
-      </c>
-      <c r="D89" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89" t="s">
-        <v>8</v>
-      </c>
-      <c r="F89" t="s">
-        <v>9</v>
-      </c>
-      <c r="G89" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2745,25 +2745,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
@@ -2860,25 +2860,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -2892,7 +2892,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -2924,7 +2924,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -2956,7 +2956,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
@@ -3071,25 +3071,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>80</v>
@@ -3135,7 +3135,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>80</v>
@@ -3186,25 +3186,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -3269,25 +3269,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -3301,7 +3301,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -3313,7 +3313,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>21</v>
@@ -3352,25 +3352,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -3449,25 +3449,25 @@
     <row r="4" spans="1:10"/>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>70</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>70</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -3609,7 +3609,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>70</v>
@@ -3692,25 +3692,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -3756,7 +3756,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -3788,7 +3788,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -3820,7 +3820,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3852,7 +3852,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -3884,7 +3884,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -3916,7 +3916,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -3949,25 +3949,25 @@
     <row r="9" spans="1:10"/>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -4046,25 +4046,25 @@
     <row r="13" spans="1:10"/>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="F14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
         <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
@@ -4078,7 +4078,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>32</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
@@ -4302,7 +4302,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
@@ -4334,7 +4334,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
@@ -4367,25 +4367,25 @@
     <row r="24" spans="1:10"/>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="F25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
+      <c r="G25" t="s">
         <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" t="s">
-        <v>10</v>
       </c>
       <c r="H25" t="s">
         <v>11</v>
@@ -4399,7 +4399,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>42</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
         <v>42</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
         <v>42</v>
@@ -4496,25 +4496,25 @@
     <row r="29" spans="1:10"/>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" t="s">
+      <c r="F30" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
+      <c r="G30" t="s">
         <v>6</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" t="s">
-        <v>10</v>
       </c>
       <c r="H30" t="s">
         <v>11</v>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
         <v>46</v>
@@ -4561,25 +4561,25 @@
     <row r="32" spans="1:10"/>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
+      <c r="F33" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
+      <c r="G33" t="s">
         <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
-        <v>10</v>
       </c>
       <c r="H33" t="s">
         <v>11</v>
@@ -4593,7 +4593,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
@@ -4657,7 +4657,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
@@ -4690,25 +4690,25 @@
     <row r="37" spans="1:10"/>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
+      <c r="F38" t="s">
         <v>5</v>
       </c>
-      <c r="C38" t="s">
+      <c r="G38" t="s">
         <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" t="s">
-        <v>10</v>
       </c>
       <c r="H38" t="s">
         <v>11</v>
@@ -4722,7 +4722,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
         <v>52</v>
@@ -4754,7 +4754,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
         <v>52</v>
@@ -4787,25 +4787,25 @@
     <row r="41" spans="1:10"/>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" t="s">
+      <c r="F42" t="s">
         <v>5</v>
       </c>
-      <c r="C42" t="s">
+      <c r="G42" t="s">
         <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" t="s">
-        <v>8</v>
-      </c>
-      <c r="F42" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" t="s">
-        <v>10</v>
       </c>
       <c r="H42" t="s">
         <v>11</v>
@@ -4819,7 +4819,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
         <v>55</v>

</xml_diff>